<commit_message>
Added graph to excel sheet
</commit_message>
<xml_diff>
--- a/concepts/GestationalData.xlsx
+++ b/concepts/GestationalData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
-  <si>
-    <t>Gestational Age</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Length (inches)</t>
   </si>
@@ -44,220 +41,115 @@
     <t>Mass (g)</t>
   </si>
   <si>
-    <t>8 weeks</t>
-  </si>
-  <si>
     <t>0.04 oz</t>
   </si>
   <si>
-    <t>9 weeks</t>
-  </si>
-  <si>
     <t>0.07 oz</t>
   </si>
   <si>
-    <t>10 weeks</t>
-  </si>
-  <si>
     <t>0.14 oz</t>
   </si>
   <si>
-    <t>11 weeks</t>
-  </si>
-  <si>
     <t>0.25 oz</t>
   </si>
   <si>
-    <t>12 weeks</t>
-  </si>
-  <si>
     <t>0.49 oz</t>
   </si>
   <si>
-    <t>13 weeks</t>
-  </si>
-  <si>
     <t>0.81 oz</t>
   </si>
   <si>
-    <t>14 weeks</t>
-  </si>
-  <si>
     <t>1.52 oz</t>
   </si>
   <si>
-    <t>15 weeks</t>
-  </si>
-  <si>
     <t>2.47 oz</t>
   </si>
   <si>
-    <t>16 weeks</t>
-  </si>
-  <si>
     <t>3.53 oz</t>
   </si>
   <si>
-    <t>17 weeks</t>
-  </si>
-  <si>
     <t>4.94 oz</t>
   </si>
   <si>
-    <t>18 weeks</t>
-  </si>
-  <si>
     <t>6.70 oz</t>
   </si>
   <si>
-    <t>19 weeks</t>
-  </si>
-  <si>
     <t>8.47 oz</t>
   </si>
   <si>
-    <t>20 weeks</t>
-  </si>
-  <si>
     <t>10.58 oz</t>
   </si>
   <si>
-    <t>21 weeks</t>
-  </si>
-  <si>
     <t>12.70 oz</t>
   </si>
   <si>
-    <t>22 weeks</t>
-  </si>
-  <si>
     <t>15.17 oz</t>
   </si>
   <si>
-    <t>23 weeks</t>
-  </si>
-  <si>
     <t>1.10 lb</t>
   </si>
   <si>
-    <t>24 weeks</t>
-  </si>
-  <si>
     <t>1.32 lb</t>
   </si>
   <si>
-    <t>25 weeks</t>
-  </si>
-  <si>
     <t>1.46 lb</t>
   </si>
   <si>
-    <t>26 weeks</t>
-  </si>
-  <si>
     <t>1.68 lb</t>
   </si>
   <si>
-    <t>27 weeks</t>
-  </si>
-  <si>
     <t>1.93 lb</t>
   </si>
   <si>
-    <t>28 weeks</t>
-  </si>
-  <si>
     <t>2.22 lb</t>
   </si>
   <si>
-    <t>29 weeks</t>
-  </si>
-  <si>
     <t>2.54 lb</t>
   </si>
   <si>
-    <t>30 weeks</t>
-  </si>
-  <si>
     <t>2.91 lb</t>
   </si>
   <si>
-    <t>31 weeks</t>
-  </si>
-  <si>
     <t>3.31 lb</t>
   </si>
   <si>
-    <t>32 weeks</t>
-  </si>
-  <si>
     <t>3.75 lb</t>
   </si>
   <si>
-    <t>33 weeks</t>
-  </si>
-  <si>
     <t>4.23 lb</t>
   </si>
   <si>
-    <t>34 weeks</t>
-  </si>
-  <si>
     <t>4.73 lb</t>
   </si>
   <si>
-    <t>35 weeks</t>
-  </si>
-  <si>
     <t>5.25 lb</t>
   </si>
   <si>
-    <t>36 weeks</t>
-  </si>
-  <si>
     <t>5.78 lb</t>
   </si>
   <si>
-    <t>37 weeks</t>
-  </si>
-  <si>
     <t>6.30 lb</t>
   </si>
   <si>
-    <t>38 weeks</t>
-  </si>
-  <si>
     <t>6.80 lb</t>
   </si>
   <si>
-    <t>39 weeks</t>
-  </si>
-  <si>
     <t>7.25 lb</t>
   </si>
   <si>
-    <t>40 weeks</t>
-  </si>
-  <si>
     <t>7.63 lb</t>
   </si>
   <si>
-    <t>41 weeks</t>
-  </si>
-  <si>
     <t>7.93 lb</t>
   </si>
   <si>
-    <t>42 weeks</t>
-  </si>
-  <si>
     <t>8.12 lb</t>
   </si>
   <si>
-    <t>43 weeks</t>
-  </si>
-  <si>
     <t>8.19 lb</t>
+  </si>
+  <si>
+    <t>Gestational Age (weeks)</t>
   </si>
 </sst>
 </file>
@@ -322,6 +214,1134 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mass (g) Over</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Gestational Period</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mass (g)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>660.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>760.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>875.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1005.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1153.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1319.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1502.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1702.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1918.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2146.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2383.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2622.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2859.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3083.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3288.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3462.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3597.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3685.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3717.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2140286960"/>
+        <c:axId val="2097481984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2140286960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2097481984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2097481984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2140286960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,12 +1610,12 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E37"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
@@ -603,30 +1623,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="1">
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>0.63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>1.6</v>
@@ -636,14 +1656,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="1">
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>0.9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>2.2999999999999998</v>
@@ -653,14 +1673,14 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
+      <c r="A4" s="1">
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>1.22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>3.1</v>
@@ -670,14 +1690,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1">
         <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>1.61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
         <v>4.0999999999999996</v>
@@ -687,14 +1707,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
+      <c r="A6" s="1">
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>2.13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>5.4</v>
@@ -704,14 +1724,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
+      <c r="A7" s="1">
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>2.19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>7.4</v>
@@ -721,14 +1741,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
+      <c r="A8" s="1">
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>3.42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>8.6999999999999993</v>
@@ -738,14 +1758,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
+      <c r="A9" s="1">
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>3.98</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2">
         <v>10.1</v>
@@ -755,14 +1775,14 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
+      <c r="A10" s="1">
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>4.57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2">
         <v>11.6</v>
@@ -772,14 +1792,14 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
+      <c r="A11" s="1">
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>5.12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2">
         <v>13</v>
@@ -789,14 +1809,14 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
+      <c r="A12" s="1">
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>5.59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2">
         <v>14.2</v>
@@ -806,14 +1826,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
+      <c r="A13" s="1">
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>6.02</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2">
         <v>15.3</v>
@@ -823,14 +1843,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
+      <c r="A14" s="1">
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>6.46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2">
         <v>16.399999999999999</v>
@@ -840,14 +1860,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
+      <c r="A15" s="1">
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>10.51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>26.7</v>
@@ -857,14 +1877,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
+      <c r="A16" s="1">
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>10.94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
         <v>27.8</v>
@@ -874,14 +1894,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
+      <c r="A17" s="1">
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <v>11.38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2">
         <v>28.9</v>
@@ -891,14 +1911,14 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
+      <c r="A18" s="1">
+        <v>24</v>
       </c>
       <c r="B18" s="2">
         <v>11.81</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2">
         <v>30</v>
@@ -908,14 +1928,14 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
+      <c r="A19" s="1">
+        <v>25</v>
       </c>
       <c r="B19" s="2">
         <v>13.62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2">
         <v>34.6</v>
@@ -925,14 +1945,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
+      <c r="A20" s="1">
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <v>14.02</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2">
         <v>35.6</v>
@@ -942,14 +1962,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
+      <c r="A21" s="1">
+        <v>27</v>
       </c>
       <c r="B21" s="2">
         <v>14.41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2">
         <v>36.6</v>
@@ -959,14 +1979,14 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>45</v>
+      <c r="A22" s="1">
+        <v>28</v>
       </c>
       <c r="B22" s="2">
         <v>14.8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2">
         <v>37.6</v>
@@ -976,14 +1996,14 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>47</v>
+      <c r="A23" s="1">
+        <v>29</v>
       </c>
       <c r="B23" s="2">
         <v>15.2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2">
         <v>38.6</v>
@@ -993,14 +2013,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>49</v>
+      <c r="A24" s="1">
+        <v>30</v>
       </c>
       <c r="B24" s="2">
         <v>15.71</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2">
         <v>39.9</v>
@@ -1010,14 +2030,14 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>51</v>
+      <c r="A25" s="1">
+        <v>31</v>
       </c>
       <c r="B25" s="2">
         <v>16.18</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2">
         <v>41.1</v>
@@ -1027,14 +2047,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>53</v>
+      <c r="A26" s="1">
+        <v>32</v>
       </c>
       <c r="B26" s="2">
         <v>16.190000000000001</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2">
         <v>42.4</v>
@@ -1044,14 +2064,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>55</v>
+      <c r="A27" s="1">
+        <v>33</v>
       </c>
       <c r="B27" s="2">
         <v>17.2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D27" s="2">
         <v>43.7</v>
@@ -1061,14 +2081,14 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
+      <c r="A28" s="1">
+        <v>34</v>
       </c>
       <c r="B28" s="2">
         <v>17.72</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2">
         <v>45</v>
@@ -1078,14 +2098,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>59</v>
+      <c r="A29" s="1">
+        <v>35</v>
       </c>
       <c r="B29" s="2">
         <v>18.190000000000001</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D29" s="2">
         <v>46.2</v>
@@ -1095,14 +2115,14 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
+      <c r="A30" s="1">
+        <v>36</v>
       </c>
       <c r="B30" s="2">
         <v>18.66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2">
         <v>47.4</v>
@@ -1112,14 +2132,14 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>63</v>
+      <c r="A31" s="1">
+        <v>37</v>
       </c>
       <c r="B31" s="2">
         <v>19.13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D31" s="2">
         <v>48.6</v>
@@ -1129,14 +2149,14 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>65</v>
+      <c r="A32" s="1">
+        <v>38</v>
       </c>
       <c r="B32" s="2">
         <v>19.61</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D32" s="2">
         <v>49.8</v>
@@ -1146,14 +2166,14 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>67</v>
+      <c r="A33" s="1">
+        <v>39</v>
       </c>
       <c r="B33" s="2">
         <v>19.96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="D33" s="2">
         <v>50.7</v>
@@ -1163,14 +2183,14 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>69</v>
+      <c r="A34" s="1">
+        <v>40</v>
       </c>
       <c r="B34" s="2">
         <v>20.16</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D34" s="2">
         <v>51.2</v>
@@ -1180,14 +2200,14 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>71</v>
+      <c r="A35" s="1">
+        <v>41</v>
       </c>
       <c r="B35" s="2">
         <v>20.350000000000001</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D35" s="2">
         <v>51.7</v>
@@ -1197,14 +2217,14 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>73</v>
+      <c r="A36" s="1">
+        <v>42</v>
       </c>
       <c r="B36" s="2">
         <v>20.28</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2">
         <v>51.5</v>
@@ -1214,14 +2234,14 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>75</v>
+      <c r="A37" s="1">
+        <v>43</v>
       </c>
       <c r="B37" s="2">
         <v>20.2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D37" s="2">
         <v>51.3</v>
@@ -1232,5 +2252,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>